<commit_message>
Fixes almost all errors claimed by QA report regarding id/url missmatch
The remain errors cannot be fixed because the publisher cannot resolve
the canonical url used by the StructureMap as source and target. Because
this resource will be refactored using FSH Mapping, the errors are
ignored.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Q4MSArztbriefProfile.xlsx
+++ b/output/StructureDefinition-Q4MSArztbriefProfile.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://qpath4ms.ukdd.de/fhir/StructureDefinition/q4ms-arztbrief</t>
+    <t>http://qpath4ms.ukdd.de/fhir/StructureDefinition/Q4MSArztbriefProfile</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-01-13T14:43:39+01:00</t>
+    <t>2022-01-19T20:56:59+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -108,7 +108,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://qpath4ms.ukdd.de/fhir/StructureDefinition/q4ms-dokument</t>
+    <t>http://qpath4ms.ukdd.de/fhir/StructureDefinition/Q4MSDokumentProfile</t>
   </si>
   <si>
     <t>Abstract</t>
@@ -1624,48 +1624,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="44.51171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="46.234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="70.24609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="73.23046875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="70.828125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="57.9296875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="42.26171875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="73.8125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="56.99609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="44.06640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="26.6875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="50.640625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="29.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="52.00390625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="33.046875" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="81.6875" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="155.4375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="84.22265625" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="162.4453125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Fixes missing name warnings with regard to ActivityDefinition resources
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Q4MSArztbriefProfile.xlsx
+++ b/output/StructureDefinition-Q4MSArztbriefProfile.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-01-19T20:56:59+01:00</t>
+    <t>2022-01-20T13:58:01+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1624,48 +1624,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="46.234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="44.51171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="73.23046875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="70.24609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="73.8125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="56.99609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="44.06640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="70.828125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="57.9296875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="42.26171875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="29.69921875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="52.00390625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="26.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="50.640625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="84.22265625" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="162.4453125" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="33.046875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="81.6875" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="155.4375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Adds CarePlan examples (again) after fixing recursive declaration error
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Q4MSArztbriefProfile.xlsx
+++ b/output/StructureDefinition-Q4MSArztbriefProfile.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-01-20T13:58:01+01:00</t>
+    <t>2022-01-20T14:56:11+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1624,48 +1624,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="44.51171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="46.234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="70.24609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="73.23046875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="70.828125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="57.9296875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="42.26171875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="73.8125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="56.99609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="44.06640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="26.6875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="50.640625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="29.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="52.00390625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="33.046875" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="81.6875" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="155.4375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="84.22265625" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="162.4453125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>